<commit_message>
Fill-in Gantt Chart (`PHW3S.xlsx`), update group notebook `_PHW3S/Exercises.ipynb`, add my notebook `PHW3S.ipynb` and video `VIDEO.zip`
</commit_message>
<xml_diff>
--- a/Daniel Gargiullo/PHW3S/PHW3S.xlsx
+++ b/Daniel Gargiullo/PHW3S/PHW3S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\DataGripProjects\Group_2_CSCI381\Daniel Gargiullo\PHW3S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{338E44E9-4A3C-42D9-9CF9-A36D0369498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D64222B-7A48-4215-8AFD-4CB5A5B1DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,10 +165,10 @@
     <t>10 Propositions</t>
   </si>
   <si>
-    <t>Study Ch. 4 &amp; 5 Content</t>
-  </si>
-  <si>
-    <t>Complete Examples from Ch. 4 &amp; 5</t>
+    <t>Study Ch. 6 Content</t>
+  </si>
+  <si>
+    <t>Complete Exercises from Ch. 6</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <dimension ref="B1:BO29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1310,7 +1310,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="7">
         <v>4</v>
@@ -1327,10 +1327,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7">
         <v>6</v>
@@ -1344,7 +1344,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="7">
         <v>6</v>
@@ -1353,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="8">
         <v>1</v>
@@ -1367,13 +1367,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
@@ -1384,13 +1384,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
         <v>2</v>
-      </c>
-      <c r="E9" s="7">
-        <v>3</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>

</xml_diff>